<commit_message>
updated ML model performance spreadsheet
</commit_message>
<xml_diff>
--- a/misc/tables_and_other/ML_model_performance.xlsx
+++ b/misc/tables_and_other/ML_model_performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\werne\GitHub\point_cloud_vegetation_filtering\misc\tables_and_other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6671494b26eed502/Documents/GitHub/point_cloud_vegetation_filtering/misc/tables_and_other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDA147A-C41E-4D84-A055-FE4E0D1E7874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{0DDA147A-C41E-4D84-A055-FE4E0D1E7874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACC6D2FA-9823-4E9A-A5C6-FBEE8B22B54F}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{8DCF5AFF-D886-48A3-80E0-141B4EF1DBE8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{8DCF5AFF-D886-48A3-80E0-141B4EF1DBE8}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="classification_analysis" sheetId="3" r:id="rId4"/>
     <sheet name="computing_cloud_metrics" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -486,11 +486,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -691,14 +691,14 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -718,16 +718,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -762,6 +762,7 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,7 +790,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -42504,9 +42504,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -42544,7 +42544,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -42650,7 +42650,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -42792,7 +42792,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -42802,61 +42802,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F6A66E-88A0-4AD5-8234-0F09C8AD5240}">
   <dimension ref="A1:AP43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.41796875" customWidth="1"/>
-    <col min="4" max="4" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1015625" customWidth="1"/>
-    <col min="21" max="21" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.41796875" style="15" customWidth="1"/>
-    <col min="24" max="24" width="9.1015625" style="15"/>
-    <col min="25" max="25" width="14.89453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.3125" style="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.1015625" style="15"/>
-    <col min="28" max="28" width="12.3125" style="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.3125" style="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.5234375" style="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.1015625" style="15" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.89453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.3125" style="15" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.1015625" style="15" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.3125" style="15" bestFit="1" customWidth="1"/>
-    <col min="36" max="39" width="9.1015625" style="15"/>
-    <col min="40" max="40" width="11.1015625" style="15" customWidth="1"/>
-    <col min="41" max="41" width="9.1015625" style="15"/>
-    <col min="42" max="42" width="12.3125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.08984375" customWidth="1"/>
+    <col min="21" max="21" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.453125" style="15" customWidth="1"/>
+    <col min="24" max="24" width="9.08984375" style="15"/>
+    <col min="25" max="25" width="14.90625" style="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.08984375" style="15"/>
+    <col min="28" max="28" width="12.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.90625" style="15" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="36" max="39" width="9.08984375" style="15"/>
+    <col min="40" max="40" width="11.08984375" style="15" customWidth="1"/>
+    <col min="41" max="41" width="9.08984375" style="15"/>
+    <col min="42" max="42" width="12.26953125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="33">
         <v>0.88724999999999998</v>
       </c>
@@ -42866,12 +42866,12 @@
       <c r="H2" s="34"/>
       <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="33">
         <v>2.8186100000000001</v>
       </c>
@@ -42881,7 +42881,7 @@
       <c r="H3" s="34"/>
       <c r="I3" s="33"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>59</v>
       </c>
@@ -42894,13 +42894,13 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -42928,7 +42928,7 @@
         <v>-4.07676 +/- 3.15798</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -42956,29 +42956,29 @@
         <v>2.49867 +/- 2.31663</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
       <c r="W8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AE8" s="50" t="s">
+      <c r="AE8" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="AF8" s="50"/>
-      <c r="AG8" s="50"/>
-      <c r="AH8" s="50"/>
-      <c r="AI8" s="50"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -43062,7 +43062,7 @@
         <v>Total Params</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>1</v>
       </c>
@@ -43088,12 +43088,12 @@
         <f>SUBSTITUTE(AD10,"model_","")</f>
         <v>rgb_16</v>
       </c>
-      <c r="R10" s="49" t="s">
+      <c r="R10" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="49"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
       <c r="W10" s="16">
         <v>1</v>
       </c>
@@ -43118,14 +43118,14 @@
       <c r="AD10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AM10" s="50" t="s">
+      <c r="AM10" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="AN10" s="50"/>
-      <c r="AO10" s="50"/>
-      <c r="AP10" s="50"/>
+      <c r="AN10" s="51"/>
+      <c r="AO10" s="51"/>
+      <c r="AP10" s="51"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>2</v>
       </c>
@@ -43206,7 +43206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>3</v>
       </c>
@@ -43295,7 +43295,7 @@
         <v>155.66666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>4</v>
       </c>
@@ -43384,7 +43384,7 @@
         <v>715.66666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B14" s="7">
         <v>5</v>
       </c>
@@ -43473,7 +43473,7 @@
         <v>2859.6666666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B15" s="9">
         <v>6</v>
       </c>
@@ -43602,7 +43602,7 @@
         <v>11243.666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>1</v>
       </c>
@@ -43701,7 +43701,7 @@
         <v>44395.666666666664</v>
       </c>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
         <v>2</v>
       </c>
@@ -43800,7 +43800,7 @@
         <v>176235.66666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B18" s="7">
         <v>3</v>
       </c>
@@ -43861,7 +43861,7 @@
       <c r="AH18" s="24"/>
       <c r="AI18" s="24"/>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B19" s="7">
         <v>4</v>
       </c>
@@ -43960,7 +43960,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>5</v>
       </c>
@@ -44059,7 +44059,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B21" s="9">
         <v>6</v>
       </c>
@@ -44188,7 +44188,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>1</v>
       </c>
@@ -44245,7 +44245,7 @@
       <c r="AH22" s="24"/>
       <c r="AI22" s="24"/>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B23" s="7">
         <v>2</v>
       </c>
@@ -44302,7 +44302,7 @@
       <c r="AH23" s="24"/>
       <c r="AI23" s="24"/>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>3</v>
       </c>
@@ -44359,7 +44359,7 @@
       <c r="AH24" s="24"/>
       <c r="AI24" s="24"/>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B25" s="7">
         <v>4</v>
       </c>
@@ -44416,7 +44416,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B26" s="7">
         <v>5</v>
       </c>
@@ -44473,7 +44473,7 @@
       <c r="AH26" s="24"/>
       <c r="AI26" s="24"/>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B27" s="9">
         <v>6</v>
       </c>
@@ -44564,7 +44564,7 @@
         <v>39353</v>
       </c>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B28" s="4">
         <v>2</v>
       </c>
@@ -44621,7 +44621,7 @@
       <c r="AH28" s="24"/>
       <c r="AI28" s="24"/>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B29" s="7">
         <v>2</v>
       </c>
@@ -44678,7 +44678,7 @@
       <c r="AH29" s="24"/>
       <c r="AI29" s="24"/>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B30" s="9">
         <v>2</v>
       </c>
@@ -44769,7 +44769,7 @@
         <v>427.66666666666669</v>
       </c>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
         <v>3</v>
       </c>
@@ -44826,7 +44826,7 @@
       <c r="AH31" s="24"/>
       <c r="AI31" s="24"/>
     </row>
-    <row r="32" spans="2:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:42" x14ac:dyDescent="0.35">
       <c r="B32" s="7">
         <v>3</v>
       </c>
@@ -44883,7 +44883,7 @@
       <c r="AH32" s="24"/>
       <c r="AI32" s="24"/>
     </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B33" s="9">
         <v>3</v>
       </c>
@@ -44974,7 +44974,7 @@
         <v>699.66666666666663</v>
       </c>
     </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>2</v>
       </c>
@@ -45031,7 +45031,7 @@
       <c r="AH34" s="24"/>
       <c r="AI34" s="24"/>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B35" s="7">
         <v>2</v>
       </c>
@@ -45088,7 +45088,7 @@
       <c r="AH35" s="24"/>
       <c r="AI35" s="24"/>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B36" s="9">
         <v>2</v>
       </c>
@@ -45179,7 +45179,7 @@
         <v>150.33333333333334</v>
       </c>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <v>3</v>
       </c>
@@ -45236,7 +45236,7 @@
       <c r="AH37" s="24"/>
       <c r="AI37" s="24"/>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B38" s="7">
         <v>3</v>
       </c>
@@ -45293,7 +45293,7 @@
       <c r="AH38" s="24"/>
       <c r="AI38" s="24"/>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B39" s="9">
         <v>3</v>
       </c>
@@ -45384,7 +45384,7 @@
         <v>222.33333333333334</v>
       </c>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B40" s="7">
         <v>3</v>
       </c>
@@ -45428,7 +45428,7 @@
       <c r="AH40" s="24"/>
       <c r="AI40" s="24"/>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B41" s="9">
         <v>3</v>
       </c>
@@ -45487,7 +45487,7 @@
       <c r="AH41" s="24"/>
       <c r="AI41" s="24"/>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B42" s="7">
         <v>3</v>
       </c>
@@ -45531,7 +45531,7 @@
       <c r="AH42" s="24"/>
       <c r="AI42" s="24"/>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.35">
       <c r="B43" s="9">
         <v>3</v>
       </c>
@@ -45601,6 +45601,18 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
   </mergeCells>
+  <conditionalFormatting sqref="D10:D39">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F10:F39">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -45610,18 +45622,6 @@
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D39">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -45659,37 +45659,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9EEADE-EB92-49D2-AC21-19FD28E12729}">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="C117" workbookViewId="0">
+      <selection activeCell="N130" sqref="N130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.41796875" customWidth="1"/>
-    <col min="4" max="4" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1015625" customWidth="1"/>
-    <col min="21" max="21" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.08984375" customWidth="1"/>
+    <col min="21" max="21" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
       <c r="J1" t="s">
         <v>67</v>
       </c>
@@ -45700,12 +45700,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="33">
         <v>0.88724999999999998</v>
       </c>
@@ -45722,12 +45722,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="33">
         <v>2.8186100000000001</v>
       </c>
@@ -45744,7 +45744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>59</v>
       </c>
@@ -45757,11 +45757,11 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
       <c r="J4">
         <v>3</v>
       </c>
@@ -45770,7 +45770,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -45805,7 +45805,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -45840,7 +45840,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="J7">
         <v>6</v>
       </c>
@@ -45849,19 +45849,19 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -45907,7 +45907,7 @@
         <v>Total Params</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>16</v>
       </c>
@@ -45935,14 +45935,14 @@
       <c r="I10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="R10" s="49" t="s">
+      <c r="R10" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="49"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>A10+16*POWER(2,B11-1)</f>
         <v>48</v>
@@ -45987,7 +45987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" ref="A12:A15" si="2">A11+16*POWER(2,B12-1)</f>
         <v>112</v>
@@ -46036,7 +46036,7 @@
         <v>155.66666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>240</v>
@@ -46085,7 +46085,7 @@
         <v>715.66666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>496</v>
@@ -46134,7 +46134,7 @@
         <v>2859.6666666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>1008</v>
@@ -46203,7 +46203,7 @@
         <v>11243.666666666666</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>16</v>
       </c>
@@ -46256,7 +46256,7 @@
         <v>44395.666666666664</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <f>A16+16*POWER(2,B17-1)</f>
         <v>48</v>
@@ -46310,7 +46310,7 @@
         <v>176235.66666666666</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" ref="A18:A21" si="8">A17+16*POWER(2,B18-1)</f>
         <v>112</v>
@@ -46345,7 +46345,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="8"/>
         <v>240</v>
@@ -46399,7 +46399,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="8"/>
         <v>496</v>
@@ -46453,7 +46453,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="8"/>
         <v>1008</v>
@@ -46522,7 +46522,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>16</v>
       </c>
@@ -46554,7 +46554,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <f>A22+16*POWER(2,B23-1)</f>
         <v>48</v>
@@ -46587,7 +46587,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" ref="A24:A27" si="12">A23+16*POWER(2,B24-1)</f>
         <v>112</v>
@@ -46620,7 +46620,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="12"/>
         <v>240</v>
@@ -46653,7 +46653,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="12"/>
         <v>496</v>
@@ -46686,7 +46686,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="12"/>
         <v>1008</v>
@@ -46736,7 +46736,7 @@
         <v>39353</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <f>16*B28</f>
         <v>32</v>
@@ -46769,7 +46769,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" ref="A29:A33" si="14">16*B29</f>
         <v>32</v>
@@ -46802,7 +46802,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="14"/>
         <v>32</v>
@@ -46852,7 +46852,7 @@
         <v>427.66666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <f>16*B31</f>
         <v>48</v>
@@ -46885,7 +46885,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="14"/>
         <v>48</v>
@@ -46918,7 +46918,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="14"/>
         <v>48</v>
@@ -46968,7 +46968,7 @@
         <v>699.66666666666663</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
         <f>8*B34</f>
         <v>16</v>
@@ -47001,7 +47001,7 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" ref="A35:A42" si="17">8*B35</f>
         <v>16</v>
@@ -47034,7 +47034,7 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="17"/>
         <v>16</v>
@@ -47084,7 +47084,7 @@
         <v>150.33333333333334</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="17"/>
         <v>24</v>
@@ -47117,7 +47117,7 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="17"/>
         <v>24</v>
@@ -47150,7 +47150,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="17"/>
         <v>24</v>
@@ -47200,7 +47200,7 @@
         <v>222.33333333333334</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="17"/>
         <v>24</v>
@@ -47235,7 +47235,7 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" ref="A41" si="20">16*B41</f>
         <v>48</v>
@@ -47285,7 +47285,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="17"/>
         <v>24</v>
@@ -47320,7 +47320,7 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" ref="A43" si="21">16*B43</f>
         <v>48</v>
@@ -47370,15 +47370,15 @@
         <v>417</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="58">
+      <c r="D44" s="49">
         <f>AVERAGE(D10:D43)</f>
         <v>0.90956470588235305</v>
       </c>
-      <c r="E44" s="58">
+      <c r="E44" s="49">
         <f>AVERAGE(E10:E43)</f>
         <v>0.91212647058823537</v>
       </c>
@@ -47388,7 +47388,7 @@
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J45" s="1"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -47404,6 +47404,18 @@
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="J8:N8"/>
   </mergeCells>
+  <conditionalFormatting sqref="D10:D39">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F10:F39">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -47413,18 +47425,6 @@
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D39">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -47439,43 +47439,43 @@
   <dimension ref="A1:V45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.68359375" customWidth="1"/>
-    <col min="6" max="6" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.7890625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.20703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="54"/>
       <c r="G1" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="55"/>
-      <c r="B2" s="57"/>
+    <row r="2" spans="1:22" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="56"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
@@ -47501,7 +47501,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>analysis!I10</f>
         <v>rgb_16</v>
@@ -47540,7 +47540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>analysis!I11</f>
         <v>rgb_16_32</v>
@@ -47591,7 +47591,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>analysis!I12</f>
         <v>rgb_16_32_64</v>
@@ -47638,7 +47638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>analysis!I13</f>
         <v>rgb_16_32_64_128</v>
@@ -47685,7 +47685,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>analysis!I14</f>
         <v>rgb_16_32_64_128_256</v>
@@ -47732,7 +47732,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="30" t="str">
         <f>analysis!I15</f>
         <v>rgb_16_32_64_128_256_512</v>
@@ -47779,7 +47779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>analysis!I16</f>
         <v>rgb_simple_16</v>
@@ -47830,7 +47830,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>analysis!I17</f>
         <v>rgb_simple_16_32</v>
@@ -47877,7 +47877,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>analysis!I18</f>
         <v>rgb_simple_16_32_64</v>
@@ -47924,7 +47924,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>analysis!I19</f>
         <v>rgb_simple_16_32_64_128</v>
@@ -47971,7 +47971,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>analysis!I20</f>
         <v>rgb_simple_16_32_64_128_256</v>
@@ -48018,7 +48018,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="30" t="str">
         <f>analysis!I21</f>
         <v>rgb_simple_16_32_64_128_256_512</v>
@@ -48065,7 +48065,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>analysis!I22</f>
         <v>all_16</v>
@@ -48132,7 +48132,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>analysis!I23</f>
         <v>all_16_32</v>
@@ -48195,7 +48195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>analysis!I24</f>
         <v>all_16_32_64</v>
@@ -48258,7 +48258,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>analysis!I25</f>
         <v>all_16_32_64_128</v>
@@ -48321,7 +48321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>analysis!I26</f>
         <v>all_16_32_64_128_256</v>
@@ -48384,7 +48384,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="30" t="str">
         <f>analysis!I27</f>
         <v>all_16_32_64_128_256_512</v>
@@ -48447,7 +48447,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>analysis!I28</f>
         <v>rgb_16_16</v>
@@ -48490,7 +48490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>analysis!I29</f>
         <v>rgb_simple_16_16</v>
@@ -48533,7 +48533,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="30" t="str">
         <f>analysis!I30</f>
         <v>all_16_16</v>
@@ -48584,7 +48584,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>analysis!I31</f>
         <v>rgb_16_16_16</v>
@@ -48627,7 +48627,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>analysis!I32</f>
         <v>rgb_simple_16_16_16</v>
@@ -48678,7 +48678,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="30" t="str">
         <f>analysis!I33</f>
         <v>all_16_16_16</v>
@@ -48745,7 +48745,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>analysis!I34</f>
         <v>rgb_8_8</v>
@@ -48792,7 +48792,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>analysis!I35</f>
         <v>rgb_simple_8_8</v>
@@ -48831,7 +48831,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="30" t="str">
         <f>analysis!I36</f>
         <v>all_8_8</v>
@@ -48886,7 +48886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>analysis!I37</f>
         <v>rgb_8_8_8</v>
@@ -48925,7 +48925,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>analysis!I38</f>
         <v>rgb_simple_8_8_8</v>
@@ -48964,7 +48964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="30" t="str">
         <f>analysis!I39</f>
         <v>all_8_8_8</v>
@@ -49011,7 +49011,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f>analysis!I40</f>
         <v>xyzrgb_8_8_8</v>
@@ -49050,7 +49050,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="30" t="str">
         <f>analysis!I41</f>
         <v>xyzrgb_16_16_16</v>
@@ -49089,7 +49089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f>analysis!I42</f>
         <v>sdrgb_8_8_8</v>
@@ -49128,7 +49128,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f>analysis!I43</f>
         <v>sdrgb_16_16_16</v>
@@ -49167,7 +49167,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T37" s="42" t="s">
         <v>126</v>
       </c>
@@ -49178,7 +49178,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T38" s="42" t="s">
         <v>127</v>
       </c>
@@ -49189,7 +49189,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T39" s="42" t="s">
         <v>128</v>
       </c>
@@ -49200,7 +49200,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T40" s="42" t="s">
         <v>129</v>
       </c>
@@ -49211,7 +49211,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T41" s="42" t="s">
         <v>130</v>
       </c>
@@ -49222,7 +49222,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T42" s="42" t="s">
         <v>73</v>
       </c>
@@ -49233,7 +49233,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T43" s="40" t="s">
         <v>74</v>
       </c>
@@ -49244,7 +49244,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T44" s="40" t="s">
         <v>71</v>
       </c>
@@ -49255,7 +49255,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T45" s="40" t="s">
         <v>72</v>
       </c>
@@ -49285,35 +49285,35 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="52"/>
+      <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="29" t="s">
         <v>46</v>
       </c>
@@ -49339,7 +49339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>analysis!I10</f>
         <v>rgb_16</v>
@@ -49367,7 +49367,7 @@
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>analysis!I11</f>
         <v>rgb_16_32</v>
@@ -49395,7 +49395,7 @@
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>analysis!I12</f>
         <v>rgb_16_32_64</v>
@@ -49423,7 +49423,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>analysis!I13</f>
         <v>rgb_16_32_64_128</v>
@@ -49451,7 +49451,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>analysis!I14</f>
         <v>rgb_16_32_64_128_256</v>
@@ -49479,7 +49479,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="30" t="str">
         <f>analysis!I15</f>
         <v>rgb_16_32_64_128_256_512</v>
@@ -49507,7 +49507,7 @@
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>analysis!I16</f>
         <v>rgb_simple_16</v>
@@ -49535,7 +49535,7 @@
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>analysis!I17</f>
         <v>rgb_simple_16_32</v>
@@ -49563,7 +49563,7 @@
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>analysis!I18</f>
         <v>rgb_simple_16_32_64</v>
@@ -49591,7 +49591,7 @@
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>analysis!I19</f>
         <v>rgb_simple_16_32_64_128</v>
@@ -49619,7 +49619,7 @@
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>analysis!I20</f>
         <v>rgb_simple_16_32_64_128_256</v>
@@ -49647,7 +49647,7 @@
       <c r="G13" s="31"/>
       <c r="H13" s="31"/>
     </row>
-    <row r="14" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="30" t="str">
         <f>analysis!I21</f>
         <v>rgb_simple_16_32_64_128_256_512</v>
@@ -49675,7 +49675,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>analysis!I22</f>
         <v>all_16</v>
@@ -49707,7 +49707,7 @@
         <v>52131820</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>analysis!I23</f>
         <v>all_16_32</v>
@@ -49739,7 +49739,7 @@
         <v>57493581</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>analysis!I24</f>
         <v>all_16_32_64</v>
@@ -49771,7 +49771,7 @@
         <v>57787109</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>analysis!I25</f>
         <v>all_16_32_64_128</v>
@@ -49803,7 +49803,7 @@
         <v>59336771</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>analysis!I26</f>
         <v>all_16_32_64_128_256</v>
@@ -49835,7 +49835,7 @@
         <v>59879060</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="30" t="str">
         <f>analysis!I27</f>
         <v>all_16_32_64_128_256_512</v>
@@ -49867,7 +49867,7 @@
         <v>59699547</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>analysis!I28</f>
         <v>rgb_16_16</v>
@@ -49899,7 +49899,7 @@
         <v>57665739</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>analysis!I29</f>
         <v>rgb_simple_16_16</v>
@@ -49931,7 +49931,7 @@
         <v>58200965</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="30" t="str">
         <f>analysis!I30</f>
         <v>all_16_16</v>
@@ -49963,7 +49963,7 @@
         <v>58251287</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>analysis!I31</f>
         <v>rgb_16_16_16</v>
@@ -49995,7 +49995,7 @@
         <v>61569343</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>analysis!I32</f>
         <v>rgb_simple_16_16_16</v>
@@ -50027,7 +50027,7 @@
         <v>58463719</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="30" t="str">
         <f>analysis!I33</f>
         <v>all_16_16_16</v>
@@ -50059,7 +50059,7 @@
         <v>59446486</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>analysis!I34</f>
         <v>rgb_8_8</v>
@@ -50091,7 +50091,7 @@
         <v>58230524</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>analysis!I35</f>
         <v>rgb_simple_8_8</v>
@@ -50123,7 +50123,7 @@
         <v>55678593</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="30" t="str">
         <f>analysis!I36</f>
         <v>all_8_8</v>
@@ -50155,7 +50155,7 @@
         <v>59376311</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>analysis!I37</f>
         <v>rgb_8_8_8</v>
@@ -50187,7 +50187,7 @@
         <v>63413350</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>analysis!I38</f>
         <v>rgb_simple_8_8_8</v>
@@ -50219,7 +50219,7 @@
         <v>57954872</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>analysis!I39</f>
         <v>all_8_8_8</v>
@@ -50293,31 +50293,31 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.41796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="H1" s="49" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="H1" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -50331,7 +50331,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>250000</v>
       </c>
@@ -50345,7 +50345,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>500000</v>
       </c>
@@ -50367,7 +50367,7 @@
         <v>2.0277777777777777</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>750000</v>
       </c>
@@ -50397,7 +50397,7 @@
         <v>3.0555555555555554</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1000000</v>
       </c>
@@ -50435,25 +50435,25 @@
         <v>4.0555555555555554</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G24" s="32">
         <f t="shared" ref="G24:G26" si="2">I3/B3</f>
         <v>0.13090909090909092</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G25" s="32">
         <f t="shared" si="2"/>
         <v>0.12351945854483926</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G26" s="32">
         <f t="shared" si="2"/>
         <v>0.1206140350877193</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G27" s="32">
         <f>I6/B6</f>
         <v>0.12279226240538267</v>

</xml_diff>